<commit_message>
Index keys to match different order.
</commit_message>
<xml_diff>
--- a/demo/translations.xlsx
+++ b/demo/translations.xlsx
@@ -11,16 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>ENGLISH</t>
-  </si>
-  <si>
-    <t>FRENCH</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>nestedObject.nameOfTheArea.title</t>
   </si>
@@ -423,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="50" customWidth="1"/>
@@ -462,17 +453,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>